<commit_message>
Added test photos and created code for json file
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\gradtag\SalishGradTag.github.io\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\SalishGradTag.github.io\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04642028-5A5E-4524-865B-05E846155801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAAA321-B94D-4860-9449-15AC2040D6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{067C688B-C076-4CA9-A153-9F35F2984BAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{067C688B-C076-4CA9-A153-9F35F2984BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Action #</t>
   </si>
@@ -53,20 +53,38 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Seed</t>
-  </si>
-  <si>
     <t>Commands</t>
   </si>
   <si>
     <t>IG Sent</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Shuffle</t>
+  </si>
+  <si>
+    <t>Yash Jain</t>
+  </si>
+  <si>
+    <t>Logan Singh</t>
+  </si>
+  <si>
+    <t>Harangad Sidhu</t>
+  </si>
+  <si>
+    <t>Unix</t>
+  </si>
+  <si>
+    <t>Justin Tran</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,13 +113,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -127,8 +150,10 @@
     <tableColumn id="3" xr3:uid="{0E87B79B-13C0-447B-B275-358530BD5389}" name="Person 1"/>
     <tableColumn id="4" xr3:uid="{3A418CF8-59A1-4A2F-95BE-A32263EAEDE9}" name="Person 2"/>
     <tableColumn id="5" xr3:uid="{8D54DE67-C333-4447-9BCF-C7947AC99220}" name="Time"/>
-    <tableColumn id="6" xr3:uid="{998624BC-1CEF-4F45-BAE9-05990C0C6965}" name="Seed"/>
-    <tableColumn id="7" xr3:uid="{2C7689FB-B8D9-4328-A56A-8BCE654D4FCE}" name="IG Sent" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{998624BC-1CEF-4F45-BAE9-05990C0C6965}" name="Unix" dataDxfId="0">
+      <calculatedColumnFormula>(E2-DATE(1970,1,1))*86400</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{2C7689FB-B8D9-4328-A56A-8BCE654D4FCE}" name="IG Sent" dataDxfId="1">
       <calculatedColumnFormula>FALSE</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -453,24 +478,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A249FE2B-2D3B-4322-ACC7-3E6F153C317B}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.9140625" customWidth="1"/>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
-    <col min="4" max="4" width="11.58203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.58203125" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,97 +512,82 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="G2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45656</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F17" si="0">(E2-DATE(1970,1,1))*86400</f>
+        <v>1735516800</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45657</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1735603200</v>
+      </c>
+      <c r="M3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45292</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1704067200</v>
+      </c>
+      <c r="M4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 2 rules and day 3 elimination
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C12D459-4BB3-48F0-BA00-3D2AF93AEE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5350B6-DF83-4531-87DD-33DB0949D3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Action #</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t>Jacob Dotto</t>
+  </si>
+  <si>
+    <t>Lauren MacNeil</t>
+  </si>
+  <si>
+    <t>Ryan Edwards</t>
+  </si>
+  <si>
+    <t>Ruby Clunas</t>
+  </si>
+  <si>
+    <t>Hudson Wilson</t>
+  </si>
+  <si>
+    <t>Aderinsola Solabomi</t>
   </si>
 </sst>
 </file>
@@ -140,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -155,11 +170,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -189,6 +213,20 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,7 +557,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,26 +709,26 @@
         <v>1740400020.0000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+    <row r="7" spans="1:7" s="15" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="16">
         <v>45712</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="19">
         <v>0.87777777777777777</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="18">
         <f t="shared" si="0"/>
         <v>1740431040.0000002</v>
       </c>
@@ -712,11 +750,11 @@
         <v>45713</v>
       </c>
       <c r="F8" s="11">
-        <v>0.46875</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
-        <v>1740482100</v>
+        <v>1740480600.0000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -736,11 +774,11 @@
         <v>45713</v>
       </c>
       <c r="F9" s="11">
-        <v>0.46875</v>
+        <v>0.46319444444444446</v>
       </c>
       <c r="G9" s="13">
-        <f t="shared" ref="G9:G11" si="1">((E9+F9)-DATE(1970,1,1))*86400</f>
-        <v>1740482100</v>
+        <f t="shared" ref="G9:G14" si="1">((E9+F9)-DATE(1970,1,1))*86400</f>
+        <v>1740481619.9999998</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -767,52 +805,109 @@
         <v>1740489600</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
+    <row r="11" spans="1:7" s="15" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="16">
         <v>45713</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="17">
         <v>0.71458333333333335</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="18">
         <f t="shared" si="1"/>
         <v>1740503340</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7">
+        <v>45714</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" si="1"/>
+        <v>1740568019.9999998</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="7">
+        <v>45714</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" si="1"/>
+        <v>1740568500</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="7">
+        <v>45714</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.51666666666666672</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" si="1"/>
+        <v>1740572640.0000002</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E15" s="12"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E16" s="12"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>

</xml_diff>

<commit_message>
Day 3 week 2
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD702A4A-F741-4A35-8284-6F0E231DBD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0F5123-DFF5-4297-AF53-617010703462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t>Action #</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>Ethan Kelly</t>
+  </si>
+  <si>
+    <t>Shaya Venktes</t>
+  </si>
+  <si>
+    <t>Alex Zhou</t>
+  </si>
+  <si>
+    <t>Sarmed Bek</t>
+  </si>
+  <si>
+    <t>Jasmine Robertson-Zhou</t>
   </si>
 </sst>
 </file>
@@ -215,7 +227,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm:ss\ \t\t"/>
-    <numFmt numFmtId="166" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -246,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -265,17 +277,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -283,17 +286,8 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -303,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -332,78 +326,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,8 +386,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G33" totalsRowShown="0">
-  <autoFilter ref="A1:G33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G35" totalsRowShown="0">
+  <autoFilter ref="A1:G35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Action #"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Command"/>
@@ -725,34 +689,35 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -769,17 +734,17 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5">
         <v>42069</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="17">
+      <c r="E2" s="10">
         <v>45711</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="16">
         <v>1.6152777777777778</v>
       </c>
       <c r="G2" s="6">
@@ -791,16 +756,16 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="10">
         <v>45712</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="16">
         <v>1.4319444444444445</v>
       </c>
       <c r="G3" s="6">
@@ -812,7 +777,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -821,10 +786,10 @@
       <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="10">
         <v>45712</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="16">
         <v>1.4375</v>
       </c>
       <c r="G4" s="6">
@@ -836,7 +801,7 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -845,10 +810,10 @@
       <c r="D5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="10">
         <v>45712</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="16">
         <v>1.4624999999999999</v>
       </c>
       <c r="G5" s="6">
@@ -860,19 +825,19 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="10">
         <v>45712</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="16">
         <v>1.51875</v>
       </c>
       <c r="G6" s="6">
@@ -880,26 +845,26 @@
         <v>1740486420.0000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="14">
         <v>45712</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="17">
         <v>1.8777777777777778</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="15">
         <f t="shared" si="0"/>
         <v>1740517440.0000002</v>
       </c>
@@ -908,19 +873,19 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="10">
         <v>45713</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="16">
         <v>1.4513888888888888</v>
       </c>
       <c r="G8" s="6">
@@ -932,19 +897,19 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="10">
         <v>45713</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="16">
         <v>1.4631944444444445</v>
       </c>
       <c r="G9" s="6">
@@ -956,19 +921,19 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="10">
         <v>45713</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="16">
         <v>1.5555555555555556</v>
       </c>
       <c r="G10" s="6">
@@ -976,26 +941,26 @@
         <v>1740576000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="11" t="s">
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="14">
         <v>45713</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="17">
         <v>1.7145833333333333</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="15">
         <f t="shared" si="0"/>
         <v>1740589740</v>
       </c>
@@ -1004,19 +969,19 @@
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="10">
         <v>45714</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="16">
         <v>1.4631944444444445</v>
       </c>
       <c r="G12" s="6">
@@ -1028,19 +993,19 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="10">
         <v>45714</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="16">
         <v>1.46875</v>
       </c>
       <c r="G13" s="6">
@@ -1048,23 +1013,23 @@
         <v>1740654900</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="36">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="19">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="14">
         <v>45714</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="17">
         <v>1.5166666666666666</v>
       </c>
       <c r="G14" s="15">
@@ -1076,22 +1041,22 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="10">
         <v>45715</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="16">
         <v>1.4583333333333333</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="6">
         <f t="shared" si="0"/>
         <v>1740740400.0000002</v>
       </c>
@@ -1100,22 +1065,22 @@
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="10">
         <v>45715</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="16">
         <v>1.46875</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="6">
         <f t="shared" si="0"/>
         <v>1740741300</v>
       </c>
@@ -1124,43 +1089,43 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="10">
         <v>45715</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="16">
         <v>1.5</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="6">
         <f t="shared" si="0"/>
         <v>1740744000</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="36">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="19">
         <v>17</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="B18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="14">
         <v>45715</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="17">
         <v>1.5833333333333335</v>
       </c>
       <c r="G18" s="15">
@@ -1172,19 +1137,19 @@
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="10">
         <v>45716</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="16">
         <v>1.4520833333333334</v>
       </c>
       <c r="G19" s="6">
@@ -1196,19 +1161,19 @@
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="10">
         <v>45716</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="16">
         <v>1.4520833333333334</v>
       </c>
       <c r="G20" s="6">
@@ -1220,19 +1185,19 @@
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="10">
         <v>45716</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="16">
         <v>1.4527777777777777</v>
       </c>
       <c r="G21" s="6">
@@ -1244,19 +1209,19 @@
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="10">
         <v>45716</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="16">
         <v>1.4805555555555556</v>
       </c>
       <c r="G22" s="6">
@@ -1268,19 +1233,19 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="10">
         <v>45716</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="16">
         <v>1.5715277777777779</v>
       </c>
       <c r="G23" s="6">
@@ -1292,19 +1257,19 @@
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="10">
         <v>45716</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="16">
         <v>1.5993055555555555</v>
       </c>
       <c r="G24" s="6">
@@ -1312,48 +1277,47 @@
         <v>1740838980.0000002</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="22">
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="24" t="s">
+      <c r="B25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="14">
         <v>45716</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="17">
         <v>1.4527777777777777</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="15">
         <f t="shared" si="0"/>
         <v>1740826320</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="7">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="19">
+      <c r="E26" s="24">
         <v>45719</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="25">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="6">
         <f t="shared" si="0"/>
         <v>1741044599.9999998</v>
       </c>
@@ -1362,107 +1326,193 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="24">
         <v>45719</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="25">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="6">
         <f t="shared" si="0"/>
         <v>1741001399.9999998</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="36">
-        <v>25</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="37" t="s">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E28" s="24">
         <v>45719</v>
       </c>
-      <c r="F28" s="39">
+      <c r="F28" s="25">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G28" s="26">
-        <f t="shared" ref="G28:G30" si="1">((E28+F28)-DATE(1970,1,1))*86400</f>
+      <c r="G28" s="6">
+        <f t="shared" ref="G28:G34" si="1">((E28+F28)-DATE(1970,1,1))*86400</f>
         <v>1741005000.0000002</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="7">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="18" t="s">
+    <row r="29" spans="1:7" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20">
+        <v>31</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="21">
+        <v>45719</v>
+      </c>
+      <c r="F29" s="22">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="G29" s="15">
+        <f t="shared" si="1"/>
+        <v>1741017480</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="24">
+        <v>45720</v>
+      </c>
+      <c r="F30" s="25">
+        <v>0.4375</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="1"/>
+        <v>1741084200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
+        <v>29</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E31" s="24">
         <v>45720</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F31" s="25">
         <v>0.85</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G31" s="6">
         <f t="shared" si="1"/>
         <v>1741119839.9999998</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="18">
-        <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="18" t="s">
+    <row r="32" spans="1:7" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11">
+        <v>30</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D32" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E32" s="21">
         <v>45720</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F32" s="22">
         <v>0.70694444444444449</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G32" s="15">
         <f t="shared" si="1"/>
         <v>1741107479.9999998</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F31" s="27"/>
-      <c r="G31" s="26"/>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="7:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G33" s="6"/>
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="23">
+        <v>31</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="24">
+        <v>45721</v>
+      </c>
+      <c r="F33" s="25">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="G33" s="29">
+        <f t="shared" si="1"/>
+        <v>1741188780.0000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="18">
+        <v>32</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="23">
+        <v>112358</v>
+      </c>
+      <c r="E34" s="24">
+        <v>45721</v>
+      </c>
+      <c r="F34" s="25">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="G34" s="29">
+        <f t="shared" si="1"/>
+        <v>1741207680.0000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G35" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week 3 day 1
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BE51C3-45C8-4275-9226-67A14965B6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA48D0-10B8-4513-9A9A-2081E7625EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="109">
   <si>
     <t>Action #</t>
   </si>
@@ -330,6 +330,36 @@
   </si>
   <si>
     <t>Minh Triet Le</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag </t>
+  </si>
+  <si>
+    <t>Eliot Rogers</t>
+  </si>
+  <si>
+    <t>Alex Wates</t>
+  </si>
+  <si>
+    <t>Ethan Darby</t>
+  </si>
+  <si>
+    <t>Haley Jones</t>
+  </si>
+  <si>
+    <t>Rylee Mason</t>
+  </si>
+  <si>
+    <t>Alexis Pascual</t>
+  </si>
+  <si>
+    <t>Colton Plank</t>
+  </si>
+  <si>
+    <t>Markus Laureano</t>
+  </si>
+  <si>
+    <t>Damon Warwick</t>
   </si>
 </sst>
 </file>
@@ -537,8 +567,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G61" totalsRowShown="0">
-  <autoFilter ref="A1:G61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G66" totalsRowShown="0">
+  <autoFilter ref="A1:G66" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Action #"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Command"/>
@@ -840,10 +870,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="82" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="82" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2301,12 +2331,123 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="G61" s="6">
-        <f t="shared" si="1"/>
+        <f>((E61+F61)-DATE(1970,1,1))*86400</f>
         <v>1741561200.0000002</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G62" s="6"/>
+      <c r="A62" s="21">
+        <v>61</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E62" s="22">
+        <v>45723</v>
+      </c>
+      <c r="F62" s="24">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="G62" s="6">
+        <f t="shared" ref="G62:G66" si="3">((E62+F62)-DATE(1970,1,1))*86400</f>
+        <v>1741353480.0000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="21">
+        <v>62</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E63" s="22">
+        <v>45723</v>
+      </c>
+      <c r="F63" s="24">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="G63" s="6">
+        <f t="shared" si="3"/>
+        <v>1741353480.0000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" s="22">
+        <v>45726</v>
+      </c>
+      <c r="F64" s="24">
+        <v>0.39861111111111114</v>
+      </c>
+      <c r="G64" s="6">
+        <f t="shared" si="3"/>
+        <v>1741599239.9999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="7">
+        <v>64</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E65" s="22">
+        <v>45726</v>
+      </c>
+      <c r="F65" s="24">
+        <v>0.39097222222222222</v>
+      </c>
+      <c r="G65" s="6">
+        <f t="shared" si="3"/>
+        <v>1741598580</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>107</v>
+      </c>
+      <c r="D66" t="s">
+        <v>108</v>
+      </c>
+      <c r="E66" s="22">
+        <v>45726</v>
+      </c>
+      <c r="F66" s="24">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="G66" s="6">
+        <f t="shared" si="3"/>
+        <v>1741598820.0000002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week 3 Day 2
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA48D0-10B8-4513-9A9A-2081E7625EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4ED780-B614-4E14-987F-D381F740AA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="114">
   <si>
     <t>Action #</t>
   </si>
@@ -323,12 +323,6 @@
     <t>Miguel Flores Salceda</t>
   </si>
   <si>
-    <t>Justin Tran</t>
-  </si>
-  <si>
-    <t>Ivanilson Lopes</t>
-  </si>
-  <si>
     <t>Minh Triet Le</t>
   </si>
   <si>
@@ -360,6 +354,27 @@
   </si>
   <si>
     <t>Damon Warwick</t>
+  </si>
+  <si>
+    <t>Jared Mackie</t>
+  </si>
+  <si>
+    <t>Quinn Doiron</t>
+  </si>
+  <si>
+    <t>Olivia Osborne</t>
+  </si>
+  <si>
+    <t>Himmit Virk</t>
+  </si>
+  <si>
+    <t>Eric Mitchell</t>
+  </si>
+  <si>
+    <t>Harry Wheaton</t>
+  </si>
+  <si>
+    <t>Nate Hyland</t>
   </si>
 </sst>
 </file>
@@ -462,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -549,6 +564,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,8 +583,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G66" totalsRowShown="0">
-  <autoFilter ref="A1:G66" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G70" totalsRowShown="0">
+  <autoFilter ref="A1:G70" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Action #"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Command"/>
@@ -870,10 +886,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="82" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="82" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1572,7 +1588,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G61" si="1">((E29+F29)-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="G29:G58" si="1">((E29+F29)-DATE(1970,1,1))*86400</f>
         <v>1741005000.0000002</v>
       </c>
     </row>
@@ -1962,491 +1978,596 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E46" s="22">
         <v>45723</v>
       </c>
       <c r="F46" s="23">
-        <v>0.48055555555555557</v>
+        <v>0.15277777777777779</v>
       </c>
       <c r="G46" s="6">
         <f t="shared" si="1"/>
-        <v>1741347120.0000002</v>
+        <v>1741318800.0000002</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="7">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E47" s="22">
         <v>45723</v>
       </c>
       <c r="F47" s="23">
-        <v>6.458333333333334E-2</v>
+        <v>0.54652777777777772</v>
       </c>
       <c r="G47" s="6">
         <f t="shared" si="1"/>
-        <v>1741311180</v>
+        <v>1741352820</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E48" s="22">
         <v>45723</v>
       </c>
       <c r="F48" s="23">
-        <v>0.15277777777777779</v>
+        <v>0.54652777777777772</v>
       </c>
       <c r="G48" s="6">
         <f t="shared" si="1"/>
-        <v>1741318800.0000002</v>
+        <v>1741352820</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="7">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E49" s="22">
         <v>45723</v>
       </c>
       <c r="F49" s="23">
-        <v>0.54652777777777772</v>
+        <v>0.54097222222222219</v>
       </c>
       <c r="G49" s="6">
         <f t="shared" si="1"/>
-        <v>1741352820</v>
+        <v>1741352340.0000002</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="E50" s="22">
         <v>45723</v>
       </c>
       <c r="F50" s="23">
-        <v>0.54652777777777772</v>
+        <v>0.51597222222222228</v>
       </c>
       <c r="G50" s="6">
         <f t="shared" si="1"/>
-        <v>1741352820</v>
+        <v>1741350180</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="7">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>30</v>
+      <c r="C51" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E51" s="22">
         <v>45723</v>
       </c>
       <c r="F51" s="23">
-        <v>0.54097222222222219</v>
+        <v>0.50208333333333333</v>
       </c>
       <c r="G51" s="6">
         <f t="shared" si="1"/>
-        <v>1741352340.0000002</v>
+        <v>1741348980</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="21" t="s">
-        <v>86</v>
+      <c r="C52" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E52" s="22">
         <v>45723</v>
       </c>
       <c r="F52" s="23">
-        <v>0.51597222222222228</v>
+        <v>0.35625000000000001</v>
       </c>
       <c r="G52" s="6">
         <f t="shared" si="1"/>
-        <v>1741350180</v>
+        <v>1741336379.9999998</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="7">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>89</v>
+      <c r="C53" s="21" t="s">
+        <v>73</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E53" s="22">
         <v>45723</v>
       </c>
       <c r="F53" s="23">
-        <v>0.50208333333333333</v>
+        <v>0.55138888888888893</v>
       </c>
       <c r="G53" s="6">
         <f t="shared" si="1"/>
-        <v>1741348980</v>
+        <v>1741353240</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
+        <v>55</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="E54" s="22">
         <v>45723</v>
       </c>
       <c r="F54" s="23">
-        <v>0.35625000000000001</v>
+        <v>0.80833333333333335</v>
       </c>
       <c r="G54" s="6">
         <f t="shared" si="1"/>
-        <v>1741336379.9999998</v>
+        <v>1741375440</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="7">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E55" s="22">
         <v>45723</v>
       </c>
       <c r="F55" s="23">
-        <v>0.55138888888888893</v>
+        <v>0.46944444444444444</v>
       </c>
       <c r="G55" s="6">
         <f t="shared" si="1"/>
-        <v>1741353240</v>
+        <v>1741346160.0000002</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>53</v>
+        <v>94</v>
+      </c>
+      <c r="D56" t="s">
+        <v>93</v>
       </c>
       <c r="E56" s="22">
         <v>45723</v>
       </c>
       <c r="F56" s="23">
-        <v>0.80833333333333335</v>
+        <v>0.52291666666666703</v>
       </c>
       <c r="G56" s="6">
         <f t="shared" si="1"/>
-        <v>1741375440</v>
+        <v>1741350780.0000002</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="7">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>95</v>
+      <c r="C57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" t="s">
+        <v>66</v>
       </c>
       <c r="E57" s="22">
         <v>45723</v>
       </c>
       <c r="F57" s="23">
-        <v>0.46944444444444444</v>
+        <v>0.52152777777777781</v>
       </c>
       <c r="G57" s="6">
         <f t="shared" si="1"/>
-        <v>1741346160.0000002</v>
+        <v>1741350659.9999998</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="21" t="s">
-        <v>94</v>
+      <c r="C58" t="s">
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E58" s="22">
         <v>45723</v>
       </c>
       <c r="F58" s="23">
-        <v>0.52291666666666703</v>
+        <v>0.49166666666666664</v>
       </c>
       <c r="G58" s="6">
         <f t="shared" si="1"/>
-        <v>1741350780.0000002</v>
+        <v>1741348080.0000002</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="7">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" t="s">
-        <v>65</v>
-      </c>
-      <c r="D59" t="s">
-        <v>66</v>
+        <v>7</v>
+      </c>
+      <c r="C59" s="21">
+        <v>69420</v>
       </c>
       <c r="E59" s="22">
-        <v>45723</v>
+        <v>45725</v>
       </c>
       <c r="F59" s="23">
-        <v>0.52152777777777781</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="G59" s="6">
-        <f t="shared" si="1"/>
-        <v>1741350659.9999998</v>
+        <f>((E59+F59)-DATE(1970,1,1))*86400</f>
+        <v>1741561200.0000002</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="5">
-        <v>59</v>
+      <c r="A60" s="21">
+        <v>61</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="17" t="s">
         <v>98</v>
       </c>
       <c r="E60" s="22">
         <v>45723</v>
       </c>
-      <c r="F60" s="23">
-        <v>0.49166666666666664</v>
+      <c r="F60" s="40">
+        <v>0.5541666666666667</v>
       </c>
       <c r="G60" s="6">
-        <f t="shared" si="1"/>
-        <v>1741348080.0000002</v>
+        <f t="shared" ref="G60:G70" si="3">((E60+F60)-DATE(1970,1,1))*86400</f>
+        <v>1741353480.0000002</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="7">
-        <v>60</v>
+      <c r="A61" s="21">
+        <v>62</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="21">
-        <v>69420</v>
+        <v>10</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="E61" s="22">
-        <v>45725</v>
-      </c>
-      <c r="F61" s="23">
-        <v>0.95833333333333337</v>
+        <v>45723</v>
+      </c>
+      <c r="F61" s="40">
+        <v>0.5541666666666667</v>
       </c>
       <c r="G61" s="6">
-        <f>((E61+F61)-DATE(1970,1,1))*86400</f>
-        <v>1741561200.0000002</v>
+        <f t="shared" si="3"/>
+        <v>1741353480.0000002</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="21">
-        <v>61</v>
+      <c r="A62" s="5">
+        <v>63</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="D62" t="s">
+        <v>102</v>
       </c>
       <c r="E62" s="22">
-        <v>45723</v>
-      </c>
-      <c r="F62" s="24">
-        <v>0.5541666666666667</v>
+        <v>45726</v>
+      </c>
+      <c r="F62" s="40">
+        <v>0.39861111111111114</v>
       </c>
       <c r="G62" s="6">
-        <f t="shared" ref="G62:G66" si="3">((E62+F62)-DATE(1970,1,1))*86400</f>
-        <v>1741353480.0000002</v>
+        <f t="shared" si="3"/>
+        <v>1741599239.9999998</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="21">
-        <v>62</v>
+      <c r="A63" s="7">
+        <v>64</v>
       </c>
       <c r="B63" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="21" t="s">
-        <v>101</v>
+      <c r="C63" t="s">
+        <v>103</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E63" s="22">
-        <v>45723</v>
-      </c>
-      <c r="F63" s="24">
-        <v>0.5541666666666667</v>
+        <v>45726</v>
+      </c>
+      <c r="F63" s="40">
+        <v>0.39097222222222222</v>
       </c>
       <c r="G63" s="6">
         <f t="shared" si="3"/>
-        <v>1741353480.0000002</v>
+        <v>1741598580</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B64" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="21" t="s">
-        <v>103</v>
+      <c r="C64" t="s">
+        <v>105</v>
       </c>
       <c r="D64" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E64" s="22">
         <v>45726</v>
       </c>
-      <c r="F64" s="24">
-        <v>0.39861111111111114</v>
+      <c r="F64" s="40">
+        <v>0.39374999999999999</v>
       </c>
       <c r="G64" s="6">
         <f t="shared" si="3"/>
-        <v>1741599239.9999998</v>
+        <v>1741598820.0000002</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="7">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C65" t="s">
-        <v>105</v>
+      <c r="C65" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E65" s="22">
-        <v>45726</v>
-      </c>
-      <c r="F65" s="24">
-        <v>0.39097222222222222</v>
+        <v>45723</v>
+      </c>
+      <c r="F65" s="40">
+        <v>0.60347222222222219</v>
       </c>
       <c r="G65" s="6">
         <f t="shared" si="3"/>
-        <v>1741598580</v>
+        <v>1741357740.0000002</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C66" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="A66" s="5">
+        <v>67</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="21" t="s">
         <v>108</v>
       </c>
+      <c r="D66" s="17" t="s">
+        <v>109</v>
+      </c>
       <c r="E66" s="22">
-        <v>45726</v>
-      </c>
-      <c r="F66" s="24">
-        <v>0.39374999999999999</v>
+        <v>45727</v>
+      </c>
+      <c r="F66" s="40">
+        <v>0.5</v>
       </c>
       <c r="G66" s="6">
         <f t="shared" si="3"/>
-        <v>1741598820.0000002</v>
+        <v>1741694400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="7">
+        <v>68</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="22">
+        <v>45727</v>
+      </c>
+      <c r="F67" s="40">
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="G67" s="6">
+        <f t="shared" si="3"/>
+        <v>1741702439.9999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="7">
+        <v>69</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E68" s="22">
+        <v>45723</v>
+      </c>
+      <c r="F68" s="40">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="G68" s="6">
+        <f t="shared" si="3"/>
+        <v>1741311180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="5">
+        <v>70</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E69" s="22">
+        <v>45726</v>
+      </c>
+      <c r="F69" s="40">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="G69" s="6">
+        <f t="shared" si="3"/>
+        <v>1741574700.0000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" s="5">
+        <v>71</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E70" s="22">
+        <v>45727</v>
+      </c>
+      <c r="F70" s="40">
+        <v>0.43194444444444446</v>
+      </c>
+      <c r="G70" s="6">
+        <f t="shared" si="3"/>
+        <v>1741688519.9999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 2 Day 3 somestuff
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4ED780-B614-4E14-987F-D381F740AA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9546CED7-4C76-4B5B-86CD-4BF7B514DB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="115">
   <si>
     <t>Action #</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>Nate Hyland</t>
+  </si>
+  <si>
+    <t>William Pham</t>
   </si>
 </sst>
 </file>
@@ -888,8 +891,8 @@
   </sheetPr>
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="82" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,7 +1591,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G58" si="1">((E29+F29)-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="G29:G57" si="1">((E29+F29)-DATE(1970,1,1))*86400</f>
         <v>1741005000.0000002</v>
       </c>
     </row>
@@ -2241,86 +2244,86 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="7">
-        <v>58</v>
+      <c r="A57" s="5">
+        <v>59</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="E57" s="22">
         <v>45723</v>
       </c>
       <c r="F57" s="23">
-        <v>0.52152777777777781</v>
+        <v>0.49166666666666664</v>
       </c>
       <c r="G57" s="6">
         <f t="shared" si="1"/>
-        <v>1741350659.9999998</v>
+        <v>1741348080.0000002</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="5">
-        <v>59</v>
+      <c r="A58" s="7">
+        <v>60</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" t="s">
-        <v>96</v>
+        <v>7</v>
+      </c>
+      <c r="C58" s="21">
+        <v>69420</v>
       </c>
       <c r="E58" s="22">
+        <v>45725</v>
+      </c>
+      <c r="F58" s="23">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="G58" s="6">
+        <f>((E58+F58)-DATE(1970,1,1))*86400</f>
+        <v>1741561200.0000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="21">
+        <v>61</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" s="22">
         <v>45723</v>
       </c>
-      <c r="F58" s="23">
-        <v>0.49166666666666664</v>
-      </c>
-      <c r="G58" s="6">
-        <f t="shared" si="1"/>
-        <v>1741348080.0000002</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="7">
-        <v>60</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="21">
-        <v>69420</v>
-      </c>
-      <c r="E59" s="22">
-        <v>45725</v>
-      </c>
-      <c r="F59" s="23">
-        <v>0.95833333333333337</v>
+      <c r="F59" s="40">
+        <v>0.5541666666666667</v>
       </c>
       <c r="G59" s="6">
-        <f>((E59+F59)-DATE(1970,1,1))*86400</f>
-        <v>1741561200.0000002</v>
+        <f t="shared" ref="G59:G70" si="3">((E59+F59)-DATE(1970,1,1))*86400</f>
+        <v>1741353480.0000002</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="21">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E60" s="22">
         <v>45723</v>
@@ -2329,245 +2332,245 @@
         <v>0.5541666666666667</v>
       </c>
       <c r="G60" s="6">
-        <f t="shared" ref="G60:G70" si="3">((E60+F60)-DATE(1970,1,1))*86400</f>
+        <f t="shared" si="3"/>
         <v>1741353480.0000002</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="21">
-        <v>62</v>
+      <c r="A61" s="5">
+        <v>63</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="D61" t="s">
+        <v>102</v>
       </c>
       <c r="E61" s="22">
-        <v>45723</v>
+        <v>45726</v>
       </c>
       <c r="F61" s="40">
-        <v>0.5541666666666667</v>
+        <v>0.39861111111111114</v>
       </c>
       <c r="G61" s="6">
         <f t="shared" si="3"/>
-        <v>1741353480.0000002</v>
+        <v>1741599239.9999998</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="5">
-        <v>63</v>
+      <c r="A62" s="7">
+        <v>64</v>
       </c>
       <c r="B62" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D62" t="s">
-        <v>102</v>
+      <c r="C62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="E62" s="22">
         <v>45726</v>
       </c>
       <c r="F62" s="40">
-        <v>0.39861111111111114</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="G62" s="6">
         <f t="shared" si="3"/>
-        <v>1741599239.9999998</v>
+        <v>1741598580</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="7">
-        <v>64</v>
+      <c r="A63" s="5">
+        <v>65</v>
       </c>
       <c r="B63" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="D63" t="s">
+        <v>106</v>
       </c>
       <c r="E63" s="22">
         <v>45726</v>
       </c>
       <c r="F63" s="40">
-        <v>0.39097222222222222</v>
+        <v>0.39374999999999999</v>
       </c>
       <c r="G63" s="6">
         <f t="shared" si="3"/>
-        <v>1741598580</v>
+        <v>1741598820.0000002</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="5">
-        <v>65</v>
+      <c r="A64" s="7">
+        <v>66</v>
       </c>
       <c r="B64" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C64" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64" t="s">
-        <v>106</v>
+      <c r="C64" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>107</v>
       </c>
       <c r="E64" s="22">
-        <v>45726</v>
+        <v>45723</v>
       </c>
       <c r="F64" s="40">
-        <v>0.39374999999999999</v>
+        <v>0.60347222222222219</v>
       </c>
       <c r="G64" s="6">
         <f t="shared" si="3"/>
-        <v>1741598820.0000002</v>
+        <v>1741357740.0000002</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="7">
-        <v>66</v>
+      <c r="A65" s="5">
+        <v>67</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E65" s="22">
-        <v>45723</v>
+        <v>45727</v>
       </c>
       <c r="F65" s="40">
-        <v>0.60347222222222219</v>
+        <v>0.5</v>
       </c>
       <c r="G65" s="6">
         <f t="shared" si="3"/>
-        <v>1741357740.0000002</v>
+        <v>1741694400</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="5">
-        <v>67</v>
+      <c r="A66" s="7">
+        <v>68</v>
       </c>
       <c r="B66" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="E66" s="22">
         <v>45727</v>
       </c>
       <c r="F66" s="40">
-        <v>0.5</v>
+        <v>0.59305555555555556</v>
       </c>
       <c r="G66" s="6">
         <f t="shared" si="3"/>
-        <v>1741694400</v>
+        <v>1741702439.9999998</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="7">
-        <v>68</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="E67" s="22">
-        <v>45727</v>
+        <v>45723</v>
       </c>
       <c r="F67" s="40">
-        <v>0.59305555555555556</v>
+        <v>6.458333333333334E-2</v>
       </c>
       <c r="G67" s="6">
         <f t="shared" si="3"/>
-        <v>1741702439.9999998</v>
+        <v>1741311180</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="7">
-        <v>69</v>
+      <c r="A68" s="5">
+        <v>70</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="E68" s="22">
-        <v>45723</v>
+        <v>45726</v>
       </c>
       <c r="F68" s="40">
-        <v>6.458333333333334E-2</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="G68" s="6">
         <f t="shared" si="3"/>
-        <v>1741311180</v>
+        <v>1741574700.0000002</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E69" s="22">
-        <v>45726</v>
+        <v>45727</v>
       </c>
       <c r="F69" s="40">
-        <v>0.11458333333333333</v>
+        <v>0.43194444444444446</v>
       </c>
       <c r="G69" s="6">
         <f t="shared" si="3"/>
-        <v>1741574700.0000002</v>
+        <v>1741688519.9999998</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B70" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E70" s="22">
         <v>45727</v>
       </c>
-      <c r="F70" s="40">
-        <v>0.43194444444444446</v>
+      <c r="F70" s="24">
+        <v>0.47222222222222221</v>
       </c>
       <c r="G70" s="6">
         <f t="shared" si="3"/>
-        <v>1741688519.9999998</v>
+        <v>1741691999.9999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wall day 1 part 2
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4CA378-A0E2-49EC-9B35-61DD65A8AC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628579F5-B80C-4D9A-B4CF-F1BA224E083B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="145">
   <si>
     <t>Action #</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>Justin Tran</t>
+  </si>
+  <si>
+    <t>Mya Wiggins</t>
+  </si>
+  <si>
+    <t>Ellie Milligan</t>
   </si>
 </sst>
 </file>
@@ -671,8 +677,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G98" totalsRowShown="0">
-  <autoFilter ref="A1:G98" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G110" totalsRowShown="0">
+  <autoFilter ref="A1:G110" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Action #"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Command"/>
@@ -974,10 +980,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="111" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="111" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3009,7 +3015,7 @@
         <v>0.45208333333333334</v>
       </c>
       <c r="G86" s="6">
-        <f t="shared" ref="G86:G98" si="6">((E86+F86)-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="G86:G100" si="6">((E86+F86)-DATE(1970,1,1))*86400</f>
         <v>1741690259.9999998</v>
       </c>
     </row>
@@ -3296,6 +3302,54 @@
       <c r="G98" s="6">
         <f t="shared" si="6"/>
         <v>1743985380</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="21">
+        <v>101</v>
+      </c>
+      <c r="B99" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D99" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E99" s="22">
+        <v>45755</v>
+      </c>
+      <c r="F99" s="24">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="G99" s="6">
+        <f t="shared" si="6"/>
+        <v>1744112340.0000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="21">
+        <v>102</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D100" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E100" s="22">
+        <v>45756</v>
+      </c>
+      <c r="F100" s="24">
+        <v>0.46250000000000002</v>
+      </c>
+      <c r="G100" s="6">
+        <f t="shared" si="6"/>
+        <v>1744196760.0000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wall day 1 part 3
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628579F5-B80C-4D9A-B4CF-F1BA224E083B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1403BD84-7ECD-4FF3-9F7C-4D500F9FE102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="146">
   <si>
     <t>Action #</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>Ellie Milligan</t>
+  </si>
+  <si>
+    <t>Connor Scott</t>
   </si>
 </sst>
 </file>
@@ -980,10 +983,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="111" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3015,7 +3018,7 @@
         <v>0.45208333333333334</v>
       </c>
       <c r="G86" s="6">
-        <f t="shared" ref="G86:G100" si="6">((E86+F86)-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="G86:G101" si="6">((E86+F86)-DATE(1970,1,1))*86400</f>
         <v>1741690259.9999998</v>
       </c>
     </row>
@@ -3318,14 +3321,14 @@
         <v>143</v>
       </c>
       <c r="E99" s="22">
-        <v>45755</v>
+        <v>45754</v>
       </c>
       <c r="F99" s="24">
         <v>0.48541666666666666</v>
       </c>
       <c r="G99" s="6">
         <f t="shared" si="6"/>
-        <v>1744112340.0000002</v>
+        <v>1744025940.0000002</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
@@ -3342,14 +3345,38 @@
         <v>144</v>
       </c>
       <c r="E100" s="22">
-        <v>45756</v>
+        <v>45754</v>
       </c>
       <c r="F100" s="24">
         <v>0.46250000000000002</v>
       </c>
       <c r="G100" s="6">
         <f t="shared" si="6"/>
-        <v>1744196760.0000002</v>
+        <v>1744023960.0000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="21">
+        <v>103</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D101" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E101" s="22">
+        <v>45754</v>
+      </c>
+      <c r="F101" s="24">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G101" s="6">
+        <f t="shared" si="6"/>
+        <v>1744023600.0000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rule update & log miss
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A84443C-8AB2-4A0D-BF82-556131F7B1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AC8B0E-F904-4956-9680-DD4630F5D092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="186">
   <si>
     <t>Action #</t>
   </si>
@@ -808,9 +808,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H172" totalsRowShown="0">
-  <autoFilter ref="A1:H172" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G173" totalsRowShown="0">
+  <autoFilter ref="A1:G173" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Action #"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Command"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Para1"/>
@@ -818,7 +818,6 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Time"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Unix"/>
-    <tableColumn id="8" xr3:uid="{0F4BEB32-5145-4AB0-AD04-70A9B133DB45}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1112,10 +1111,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H171"/>
+  <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="119" workbookViewId="0">
-      <selection activeCell="E168" activeCellId="1" sqref="A170:XFD170 E168"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="119" workbookViewId="0">
+      <selection activeCell="D174" sqref="D174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4681,7 +4680,7 @@
         <v>0.60624999999999996</v>
       </c>
       <c r="G150" s="6">
-        <f t="shared" ref="G150:G169" si="7">((E150+F150)-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="G150:G173" si="7">((E150+F150)-DATE(1970,1,1))*86400</f>
         <v>1744295579.9999998</v>
       </c>
     </row>
@@ -5071,96 +5070,165 @@
         <v>169</v>
       </c>
       <c r="B167" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D167" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="E167" s="22">
         <v>45793</v>
       </c>
       <c r="F167" s="24">
-        <v>0.52638888888888891</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="G167" s="6">
         <f t="shared" si="7"/>
-        <v>1747399080</v>
+        <v>1747387380</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="5">
-        <v>170</v>
+      <c r="A168" s="21">
+        <v>169</v>
       </c>
       <c r="B168" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C168" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D168" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E168" s="22">
-        <v>45798</v>
+        <v>45793</v>
       </c>
       <c r="F168" s="24">
-        <v>0.58125000000000004</v>
+        <v>0.52638888888888891</v>
       </c>
       <c r="G168" s="6">
         <f t="shared" si="7"/>
-        <v>1747835820.0000002</v>
+        <v>1747399080</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B169" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C169" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D169" s="17" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E169" s="22">
-        <v>45797</v>
+        <v>45798</v>
       </c>
       <c r="F169" s="24">
-        <v>0.45763888888888887</v>
+        <v>0.58125000000000004</v>
       </c>
       <c r="G169" s="6">
         <f t="shared" si="7"/>
+        <v>1747835820.0000002</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="5">
+        <v>171</v>
+      </c>
+      <c r="B170" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C170" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D170" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E170" s="22">
+        <v>45797</v>
+      </c>
+      <c r="F170" s="24">
+        <v>0.45763888888888887</v>
+      </c>
+      <c r="G170" s="6">
+        <f t="shared" si="7"/>
         <v>1747738740</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="21">
+    <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="21">
         <v>172</v>
       </c>
-      <c r="B170" s="17" t="s">
+      <c r="B171" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="C170" s="21" t="s">
+      <c r="C171" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D170" s="17" t="s">
+      <c r="D171" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E170" s="22">
+      <c r="E171" s="22">
         <v>45798</v>
       </c>
-      <c r="F170" s="24">
+      <c r="F171" s="24">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G170" s="6">
-        <f t="shared" ref="G170" si="8">((E170+F170)-DATE(1970,1,1))*86400</f>
+      <c r="G171" s="6">
+        <f t="shared" ref="G171" si="8">((E171+F171)-DATE(1970,1,1))*86400</f>
         <v>1747825200.0000002</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="5"/>
+    <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A172" s="5">
+        <v>173</v>
+      </c>
+      <c r="B172" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C172" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D172" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E172" s="22">
+        <v>45778</v>
+      </c>
+      <c r="F172" s="24">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="G172" s="6">
+        <f t="shared" si="7"/>
+        <v>1746108960.0000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="21">
+        <v>174</v>
+      </c>
+      <c r="B173" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C173" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D173" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E173" s="22">
+        <v>45792</v>
+      </c>
+      <c r="F173" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G173" s="6">
+        <f t="shared" si="7"/>
+        <v>1747310400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
gtg go eat soon
</commit_message>
<xml_diff>
--- a/src/game_log.xlsx
+++ b/src/game_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD07B544-5D9F-4E1D-A78A-F05B591A5AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C4F87C-0924-426B-9C3B-0DE1BBF04DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="187">
   <si>
     <t>Action #</t>
   </si>
@@ -588,6 +588,12 @@
   </si>
   <si>
     <t>Sadie Barrell</t>
+  </si>
+  <si>
+    <t>Harbeen Sidhu</t>
+  </si>
+  <si>
+    <t>The time is wrong</t>
   </si>
 </sst>
 </file>
@@ -805,8 +811,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G173" totalsRowShown="0">
-  <autoFilter ref="A1:G173" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G180" totalsRowShown="0">
+  <autoFilter ref="A1:G180" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Action #"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Command"/>
@@ -1108,10 +1114,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H173"/>
+  <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="119" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="119" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3146,7 +3152,7 @@
         <v>0.45208333333333334</v>
       </c>
       <c r="G86" s="6">
-        <f t="shared" ref="G86:G149" si="6">((E86+F86)-DATE(1970,1,1))*86400</f>
+        <f t="shared" ref="G86:G150" si="6">((E86+F86)-DATE(1970,1,1))*86400</f>
         <v>1741690259.9999998</v>
       </c>
     </row>
@@ -4658,103 +4664,103 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="21">
+      <c r="A150" s="5">
         <v>152</v>
       </c>
       <c r="B150" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C150" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="D150" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E150" s="22">
+        <v>45793</v>
+      </c>
+      <c r="F150" s="24">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="G150" s="6">
+        <f t="shared" si="6"/>
+        <v>1747393320</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="21">
+        <v>153</v>
+      </c>
+      <c r="B151" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C151" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D150" s="17" t="s">
+      <c r="D151" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="E150" s="22">
+      <c r="E151" s="22">
         <v>45757</v>
       </c>
-      <c r="F150" s="24">
+      <c r="F151" s="24">
         <v>0.60624999999999996</v>
       </c>
-      <c r="G150" s="6">
-        <f t="shared" ref="G150:G173" si="7">((E150+F150)-DATE(1970,1,1))*86400</f>
+      <c r="G151" s="6">
+        <f t="shared" ref="G151:G175" si="7">((E151+F151)-DATE(1970,1,1))*86400</f>
         <v>1744295579.9999998</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="5">
-        <v>153</v>
-      </c>
-      <c r="B151" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C151" s="21" t="s">
+    <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="5">
+        <v>154</v>
+      </c>
+      <c r="B152" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C152" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="D151" s="21" t="s">
+      <c r="D152" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E151" s="22">
+      <c r="E152" s="22">
         <v>45782</v>
       </c>
-      <c r="F151" s="24">
+      <c r="F152" s="24">
         <v>0.50624999999999998</v>
       </c>
-      <c r="G151" s="6">
+      <c r="G152" s="6">
         <f t="shared" si="7"/>
         <v>1746446939.9999998</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="21">
-        <v>154</v>
-      </c>
-      <c r="B152" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C152" s="21" t="s">
+    <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="21">
+        <v>155</v>
+      </c>
+      <c r="B153" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D152" s="17" t="s">
+      <c r="D153" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="E152" s="22">
+      <c r="E153" s="22">
         <v>45778</v>
       </c>
-      <c r="F152" s="24">
+      <c r="F153" s="24">
         <v>0.48402777777777778</v>
       </c>
-      <c r="G152" s="6">
+      <c r="G153" s="6">
         <f t="shared" si="7"/>
         <v>1746099420</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="5">
-        <v>155</v>
-      </c>
-      <c r="B153" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C153" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D153" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E153" s="22">
-        <v>45778</v>
-      </c>
-      <c r="F153" s="24">
-        <v>0.45763888888888887</v>
-      </c>
-      <c r="G153" s="6">
-        <f t="shared" si="7"/>
-        <v>1746097140</v>
-      </c>
-    </row>
     <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="21">
+      <c r="A154" s="5">
         <v>156</v>
       </c>
       <c r="B154" s="17" t="s">
@@ -4764,7 +4770,7 @@
         <v>28</v>
       </c>
       <c r="D154" s="21" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="E154" s="22">
         <v>45778</v>
@@ -4785,20 +4791,20 @@
         <v>10</v>
       </c>
       <c r="C155" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D155" s="17" t="s">
-        <v>181</v>
+        <v>28</v>
+      </c>
+      <c r="D155" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="E155" s="22">
-        <v>45755</v>
+        <v>45778</v>
       </c>
       <c r="F155" s="24">
-        <v>0.53680555555555554</v>
+        <v>0.45763888888888887</v>
       </c>
       <c r="G155" s="6">
         <f t="shared" si="7"/>
-        <v>1744116780.0000002</v>
+        <v>1746097140</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4808,21 +4814,21 @@
       <c r="B156" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C156" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D156" s="21" t="s">
-        <v>94</v>
+      <c r="C156" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D156" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="E156" s="22">
-        <v>45783</v>
+        <v>45755</v>
       </c>
       <c r="F156" s="24">
-        <v>0.40763888888888888</v>
+        <v>0.53680555555555554</v>
       </c>
       <c r="G156" s="6">
         <f t="shared" si="7"/>
-        <v>1746524819.9999998</v>
+        <v>1744116780.0000002</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4832,21 +4838,21 @@
       <c r="B157" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C157" s="21" t="s">
-        <v>158</v>
+      <c r="C157" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D157" s="21" t="s">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="E157" s="22">
-        <v>45791</v>
+        <v>45783</v>
       </c>
       <c r="F157" s="24">
-        <v>0.46388888888888891</v>
+        <v>0.40763888888888888</v>
       </c>
       <c r="G157" s="6">
         <f t="shared" si="7"/>
-        <v>1747220880</v>
+        <v>1746524819.9999998</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4857,20 +4863,20 @@
         <v>10</v>
       </c>
       <c r="C158" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D158" s="17" t="s">
-        <v>182</v>
+        <v>158</v>
+      </c>
+      <c r="D158" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="E158" s="22">
-        <v>45790</v>
+        <v>45791</v>
       </c>
       <c r="F158" s="24">
-        <v>0.50416666666666665</v>
+        <v>0.46388888888888891</v>
       </c>
       <c r="G158" s="6">
         <f t="shared" si="7"/>
-        <v>1747137960</v>
+        <v>1747220880</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4883,162 +4889,162 @@
       <c r="C159" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="D159" s="21" t="s">
-        <v>131</v>
+      <c r="D159" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="E159" s="22">
-        <v>45791</v>
+        <v>45790</v>
       </c>
       <c r="F159" s="24">
-        <v>0.43888888888888888</v>
+        <v>0.50416666666666665</v>
       </c>
       <c r="G159" s="6">
         <f t="shared" si="7"/>
-        <v>1747218719.9999998</v>
+        <v>1747137960</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="21">
+      <c r="A160" s="5">
         <v>162</v>
       </c>
       <c r="B160" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="D160" s="17" t="s">
-        <v>158</v>
+        <v>112</v>
+      </c>
+      <c r="D160" s="21" t="s">
+        <v>131</v>
       </c>
       <c r="E160" s="22">
-        <v>45794</v>
+        <v>45791</v>
       </c>
       <c r="F160" s="24">
-        <v>0.74305555555555558</v>
+        <v>0.43888888888888888</v>
       </c>
       <c r="G160" s="6">
         <f t="shared" si="7"/>
-        <v>1747504200</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="5">
+        <v>1747218719.9999998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="21">
         <v>163</v>
       </c>
       <c r="B161" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C161" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D161" s="21" t="s">
-        <v>175</v>
+        <v>163</v>
+      </c>
+      <c r="D161" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="E161" s="22">
-        <v>45792</v>
+        <v>45794</v>
       </c>
       <c r="F161" s="24">
-        <v>0.45833333333333331</v>
+        <v>0.74305555555555558</v>
       </c>
       <c r="G161" s="6">
         <f t="shared" si="7"/>
-        <v>1747306800.0000002</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="21">
+        <v>1747504200</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="5">
         <v>164</v>
       </c>
       <c r="B162" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C162" s="21" t="s">
         <v>112</v>
       </c>
+      <c r="D162" s="21" t="s">
+        <v>175</v>
+      </c>
       <c r="E162" s="22">
         <v>45792</v>
       </c>
       <c r="F162" s="24">
-        <v>0.48194444444444445</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="G162" s="6">
         <f t="shared" si="7"/>
-        <v>1747308840</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="5">
+        <v>1747306800.0000002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="21">
         <v>165</v>
       </c>
       <c r="B163" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C163" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D163" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C163" s="21" t="s">
         <v>112</v>
       </c>
       <c r="E163" s="22">
-        <v>45797</v>
+        <v>45792</v>
       </c>
       <c r="F163" s="24">
-        <v>0.52986111111111112</v>
+        <v>0.48194444444444445</v>
       </c>
       <c r="G163" s="6">
         <f t="shared" si="7"/>
-        <v>1747744980.0000002</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="21">
+        <v>1747308840</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="5">
         <v>166</v>
       </c>
       <c r="B164" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C164" s="21" t="s">
-        <v>156</v>
+      <c r="C164" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="D164" s="17" t="s">
-        <v>183</v>
+        <v>112</v>
       </c>
       <c r="E164" s="22">
-        <v>45792</v>
+        <v>45797</v>
       </c>
       <c r="F164" s="24">
-        <v>0.59375</v>
+        <v>0.52986111111111112</v>
       </c>
       <c r="G164" s="6">
         <f t="shared" si="7"/>
-        <v>1747318500</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1747744980.0000002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="21">
         <v>167</v>
       </c>
       <c r="B165" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>39</v>
+      <c r="C165" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="D165" s="17" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="E165" s="22">
-        <v>45791</v>
+        <v>45792</v>
       </c>
       <c r="F165" s="24">
-        <v>0.39097222222222222</v>
+        <v>0.59375</v>
       </c>
       <c r="G165" s="6">
         <f t="shared" si="7"/>
-        <v>1747214580</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1747318500</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>168</v>
       </c>
@@ -5049,20 +5055,20 @@
         <v>39</v>
       </c>
       <c r="D166" s="17" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="E166" s="22">
         <v>45791</v>
       </c>
       <c r="F166" s="24">
-        <v>0.46319444444444446</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="G166" s="6">
         <f t="shared" si="7"/>
-        <v>1747220819.9999998</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1747214580</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="21">
         <v>169</v>
       </c>
@@ -5072,159 +5078,207 @@
       <c r="C167" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D167" s="21" t="s">
-        <v>127</v>
+      <c r="D167" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="E167" s="22">
-        <v>45793</v>
+        <v>45791</v>
       </c>
       <c r="F167" s="24">
-        <v>0.39097222222222222</v>
+        <v>0.46319444444444446</v>
       </c>
       <c r="G167" s="6">
         <f t="shared" si="7"/>
-        <v>1747387380</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="21">
-        <v>169</v>
+        <v>1747220819.9999998</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="5">
+        <v>170</v>
       </c>
       <c r="B168" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D168" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="E168" s="22">
         <v>45793</v>
       </c>
       <c r="F168" s="24">
-        <v>0.52638888888888891</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="G168" s="6">
         <f t="shared" si="7"/>
-        <v>1747399080</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="5">
-        <v>170</v>
+        <v>1747387380</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="21">
+        <v>171</v>
       </c>
       <c r="B169" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C169" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D169" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C169" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E169" s="22">
-        <v>45798</v>
+        <v>45793</v>
       </c>
       <c r="F169" s="24">
-        <v>0.58125000000000004</v>
+        <v>0.52638888888888891</v>
       </c>
       <c r="G169" s="6">
         <f t="shared" si="7"/>
-        <v>1747835820.0000002</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1747399080</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B170" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C170" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D170" s="17" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E170" s="22">
-        <v>45797</v>
+        <v>45798</v>
       </c>
       <c r="F170" s="24">
-        <v>0.45763888888888887</v>
+        <v>0.58125000000000004</v>
       </c>
       <c r="G170" s="6">
         <f t="shared" si="7"/>
+        <v>1747835820.0000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="21">
+        <v>173</v>
+      </c>
+      <c r="B171" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D171" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E171" s="22">
+        <v>45797</v>
+      </c>
+      <c r="F171" s="24">
+        <v>0.45763888888888887</v>
+      </c>
+      <c r="G171" s="6">
+        <f t="shared" si="7"/>
         <v>1747738740</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="21">
-        <v>172</v>
-      </c>
-      <c r="B171" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C171" s="21" t="s">
+    <row r="172" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A172" s="5">
+        <v>174</v>
+      </c>
+      <c r="B172" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C172" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D171" s="17" t="s">
+      <c r="D172" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E171" s="22">
+      <c r="E172" s="22">
         <v>45798</v>
       </c>
-      <c r="F171" s="24">
+      <c r="F172" s="24">
         <v>0.45833333333333331</v>
-      </c>
-      <c r="G171" s="6">
-        <f t="shared" ref="G171" si="8">((E171+F171)-DATE(1970,1,1))*86400</f>
-        <v>1747825200.0000002</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="5">
-        <v>173</v>
-      </c>
-      <c r="B172" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C172" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D172" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E172" s="22">
-        <v>45778</v>
-      </c>
-      <c r="F172" s="24">
-        <v>0.59444444444444444</v>
       </c>
       <c r="G172" s="6">
         <f t="shared" si="7"/>
-        <v>1746108960.0000002</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1747825200.0000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="21">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B173" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C173" s="21" t="s">
-        <v>138</v>
+        <v>30</v>
       </c>
       <c r="D173" s="21" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="E173" s="22">
-        <v>45792</v>
+        <v>45778</v>
       </c>
       <c r="F173" s="24">
-        <v>0.5</v>
+        <v>0.59444444444444444</v>
       </c>
       <c r="G173" s="6">
         <f t="shared" si="7"/>
+        <v>1746108960.0000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A174" s="5">
+        <v>176</v>
+      </c>
+      <c r="B174" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D174" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E174" s="22">
+        <v>45792</v>
+      </c>
+      <c r="F174" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G174" s="6">
+        <f t="shared" si="7"/>
         <v>1747310400</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="21">
+        <v>177</v>
+      </c>
+      <c r="B175" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E175" s="22">
+        <v>45798</v>
+      </c>
+      <c r="F175" s="24">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G175" s="6">
+        <f t="shared" si="7"/>
+        <v>1747825200.0000002</v>
+      </c>
+      <c r="H175" s="17" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>